<commit_message>
proceso final modulo usuarios
</commit_message>
<xml_diff>
--- a/database/json/errorcodes.xlsx
+++ b/database/json/errorcodes.xlsx
@@ -134,7 +134,7 @@
     <t xml:space="preserve">ERR_17</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">El usuario no tiene ningun permiso asignado</t>
   </si>
   <si>
     <t xml:space="preserve">ERR_18</t>
@@ -677,7 +677,7 @@
   <dimension ref="A1:D1100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -948,14 +948,14 @@
         <v>36</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">CONCATENATE(A18, " - ",C18)</f>
-        <v>ERR_17 -  </v>
+        <v>ERR_17 - El usuario no tiene ningun permiso asignado</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
modirficacion de error codes
</commit_message>
<xml_diff>
--- a/database/json/errorcodes.xlsx
+++ b/database/json/errorcodes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="181">
   <si>
     <t xml:space="preserve">CODE_ID</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t xml:space="preserve">ERR_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario no tiene permiso para acceder a esta seccion</t>
   </si>
   <si>
     <t xml:space="preserve">ERR_19</t>
@@ -676,8 +679,8 @@
   </sheetPr>
   <dimension ref="A1:D1100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -965,14 +968,17 @@
       <c r="B19" s="2" t="n">
         <v>400</v>
       </c>
+      <c r="C19" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="D19" s="0" t="str">
         <f aca="false">CONCATENATE(A19, " - ",C19)</f>
-        <v>ERR_18 -</v>
+        <v>ERR_18 - El usuario no tiene permiso para acceder a esta seccion</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>400</v>
@@ -984,7 +990,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>400</v>
@@ -996,7 +1002,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>400</v>
@@ -1008,7 +1014,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>400</v>
@@ -1020,7 +1026,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>400</v>
@@ -1032,7 +1038,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>400</v>
@@ -1044,7 +1050,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>400</v>
@@ -1056,7 +1062,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>400</v>
@@ -1068,7 +1074,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2" t="n">
         <v>400</v>
@@ -1080,7 +1086,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B29" s="2" t="n">
         <v>400</v>
@@ -1093,7 +1099,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>400</v>
@@ -1106,7 +1112,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B31" s="2" t="n">
         <v>400</v>
@@ -1119,7 +1125,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>400</v>
@@ -1132,7 +1138,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>400</v>
@@ -1145,7 +1151,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B34" s="2" t="n">
         <v>400</v>
@@ -1158,7 +1164,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B35" s="2" t="n">
         <v>400</v>
@@ -1171,7 +1177,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B36" s="2" t="n">
         <v>400</v>
@@ -1184,7 +1190,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B37" s="2" t="n">
         <v>400</v>
@@ -1197,7 +1203,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B38" s="2" t="n">
         <v>400</v>
@@ -1210,7 +1216,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>400</v>
@@ -1223,7 +1229,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B40" s="2" t="n">
         <v>400</v>
@@ -1236,7 +1242,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B41" s="2" t="n">
         <v>400</v>
@@ -1249,7 +1255,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B42" s="2" t="n">
         <v>400</v>
@@ -1262,7 +1268,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B43" s="2" t="n">
         <v>400</v>
@@ -1275,7 +1281,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>400</v>
@@ -1288,7 +1294,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B45" s="2" t="n">
         <v>400</v>
@@ -1301,7 +1307,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B46" s="2" t="n">
         <v>400</v>
@@ -1313,7 +1319,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B47" s="2" t="n">
         <v>400</v>
@@ -1325,7 +1331,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B48" s="2" t="n">
         <v>400</v>
@@ -1337,7 +1343,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B49" s="2" t="n">
         <v>400</v>
@@ -1349,7 +1355,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B50" s="2" t="n">
         <v>400</v>
@@ -1361,7 +1367,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B51" s="2" t="n">
         <v>400</v>
@@ -1373,7 +1379,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B52" s="2" t="n">
         <v>400</v>
@@ -1385,7 +1391,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B53" s="2" t="n">
         <v>400</v>
@@ -1397,7 +1403,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B54" s="2" t="n">
         <v>400</v>
@@ -1409,7 +1415,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B55" s="2" t="n">
         <v>400</v>
@@ -1421,7 +1427,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B56" s="2" t="n">
         <v>400</v>
@@ -1433,7 +1439,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B57" s="2" t="n">
         <v>400</v>
@@ -1445,7 +1451,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B58" s="2" t="n">
         <v>400</v>
@@ -1457,7 +1463,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B59" s="2" t="n">
         <v>400</v>
@@ -1469,7 +1475,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B60" s="2" t="n">
         <v>400</v>
@@ -1481,7 +1487,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B61" s="2" t="n">
         <v>400</v>
@@ -1493,7 +1499,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B62" s="2" t="n">
         <v>400</v>
@@ -1505,7 +1511,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B63" s="2" t="n">
         <v>400</v>
@@ -1517,7 +1523,7 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B64" s="2" t="n">
         <v>400</v>
@@ -1529,7 +1535,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B65" s="2" t="n">
         <v>400</v>
@@ -1541,7 +1547,7 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B66" s="2" t="n">
         <v>400</v>
@@ -1553,7 +1559,7 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B67" s="2" t="n">
         <v>400</v>
@@ -1565,7 +1571,7 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B68" s="2" t="n">
         <v>400</v>
@@ -1577,7 +1583,7 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B69" s="2" t="n">
         <v>400</v>
@@ -1589,7 +1595,7 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B70" s="2" t="n">
         <v>400</v>
@@ -1601,7 +1607,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B71" s="2" t="n">
         <v>400</v>
@@ -1613,7 +1619,7 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B72" s="2" t="n">
         <v>400</v>
@@ -1625,7 +1631,7 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B73" s="2" t="n">
         <v>400</v>
@@ -1637,7 +1643,7 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B74" s="2" t="n">
         <v>400</v>
@@ -1649,7 +1655,7 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B75" s="2" t="n">
         <v>400</v>
@@ -1661,7 +1667,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B76" s="2" t="n">
         <v>400</v>
@@ -1673,7 +1679,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B77" s="2" t="n">
         <v>400</v>
@@ -1685,7 +1691,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B78" s="2" t="n">
         <v>400</v>
@@ -1697,7 +1703,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B79" s="2" t="n">
         <v>400</v>
@@ -1709,7 +1715,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B80" s="2" t="n">
         <v>400</v>
@@ -1721,7 +1727,7 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B81" s="2" t="n">
         <v>400</v>
@@ -1733,7 +1739,7 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B82" s="2" t="n">
         <v>400</v>
@@ -1745,7 +1751,7 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B83" s="2" t="n">
         <v>400</v>
@@ -1757,7 +1763,7 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B84" s="2" t="n">
         <v>400</v>
@@ -1769,7 +1775,7 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B85" s="2" t="n">
         <v>400</v>
@@ -1781,7 +1787,7 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B86" s="2" t="n">
         <v>400</v>
@@ -1793,7 +1799,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B87" s="2" t="n">
         <v>400</v>
@@ -1805,7 +1811,7 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B88" s="2" t="n">
         <v>400</v>
@@ -1817,7 +1823,7 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B89" s="2" t="n">
         <v>400</v>
@@ -1829,7 +1835,7 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B90" s="2" t="n">
         <v>400</v>
@@ -1841,7 +1847,7 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B91" s="2" t="n">
         <v>400</v>
@@ -1853,7 +1859,7 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B92" s="2" t="n">
         <v>400</v>
@@ -1865,7 +1871,7 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B93" s="2" t="n">
         <v>400</v>
@@ -1877,7 +1883,7 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B94" s="2" t="n">
         <v>400</v>
@@ -1889,7 +1895,7 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B95" s="2" t="n">
         <v>400</v>
@@ -1901,7 +1907,7 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B96" s="2" t="n">
         <v>400</v>
@@ -1913,7 +1919,7 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B97" s="2" t="n">
         <v>400</v>
@@ -1925,7 +1931,7 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B98" s="2" t="n">
         <v>400</v>
@@ -1937,7 +1943,7 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B99" s="2" t="n">
         <v>400</v>
@@ -1949,7 +1955,7 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B100" s="2" t="n">
         <v>400</v>
@@ -4978,7 +4984,7 @@
   <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="A1:D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4990,16 +4996,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5007,7 +5013,7 @@
         <v>100</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5015,7 +5021,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5023,7 +5029,7 @@
         <v>102</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5031,12 +5037,12 @@
         <v>103</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B7" s="4"/>
     </row>
@@ -5045,7 +5051,7 @@
         <v>200</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5053,7 +5059,7 @@
         <v>201</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5061,7 +5067,7 @@
         <v>202</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5069,7 +5075,7 @@
         <v>203</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5077,7 +5083,7 @@
         <v>204</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5085,7 +5091,7 @@
         <v>205</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5093,7 +5099,7 @@
         <v>206</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5113,7 +5119,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B18" s="4"/>
     </row>
@@ -5122,7 +5128,7 @@
         <v>300</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5130,7 +5136,7 @@
         <v>301</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5138,7 +5144,7 @@
         <v>302</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5146,7 +5152,7 @@
         <v>303</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5154,7 +5160,7 @@
         <v>304</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5162,7 +5168,7 @@
         <v>305</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5170,7 +5176,7 @@
         <v>306</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5178,7 +5184,7 @@
         <v>307</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5186,12 +5192,12 @@
         <v>308</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B28" s="4"/>
     </row>
@@ -5200,7 +5206,7 @@
         <v>400</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5216,7 +5222,7 @@
         <v>402</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5224,7 +5230,7 @@
         <v>403</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5232,7 +5238,7 @@
         <v>404</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5240,7 +5246,7 @@
         <v>405</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5248,7 +5254,7 @@
         <v>406</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5256,7 +5262,7 @@
         <v>407</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5264,7 +5270,7 @@
         <v>408</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5272,7 +5278,7 @@
         <v>409</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5285,7 +5291,7 @@
         <v>411</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5293,7 +5299,7 @@
         <v>412</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5301,7 +5307,7 @@
         <v>413</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5309,7 +5315,7 @@
         <v>414</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5317,7 +5323,7 @@
         <v>415</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5325,7 +5331,7 @@
         <v>416</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5333,7 +5339,7 @@
         <v>417</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5346,7 +5352,7 @@
         <v>421</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5354,7 +5360,7 @@
         <v>422</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5362,7 +5368,7 @@
         <v>423</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5370,7 +5376,7 @@
         <v>424</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5383,7 +5389,7 @@
         <v>426</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5396,7 +5402,7 @@
         <v>429</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5404,7 +5410,7 @@
         <v>431</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5412,12 +5418,12 @@
         <v>451</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B58" s="4"/>
     </row>
@@ -5426,7 +5432,7 @@
         <v>500</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5434,7 +5440,7 @@
         <v>501</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5442,7 +5448,7 @@
         <v>502</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5450,7 +5456,7 @@
         <v>503</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5458,7 +5464,7 @@
         <v>504</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5466,7 +5472,7 @@
         <v>505</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5484,7 +5490,7 @@
         <v>508</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5492,7 +5498,7 @@
         <v>510</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5500,7 +5506,7 @@
         <v>511</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>